<commit_message>
Published state of ETDataset for deploy May 2023
</commit_message>
<xml_diff>
--- a/nodes_source_analyses/energy/transport/transport_van_using_electricity.converter.xlsx
+++ b/nodes_source_analyses/energy/transport/transport_van_using_electricity.converter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10116"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathijsbijkerk/Projects/etdataset/nodes_source_analyses/energy/transport/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65CA8FF2-A78A-9442-AF7D-C811F2BB135F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21D7B8B-7AF1-4140-9896-9720ABE1AB28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60160" yWindow="-18040" windowWidth="30080" windowHeight="16080" tabRatio="762" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30080" yWindow="-18040" windowWidth="30080" windowHeight="32220" tabRatio="762" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
@@ -502,7 +502,7 @@
     <t>storage decay per month</t>
   </si>
   <si>
-    <t>DC snelladen</t>
+    <t>Onboard charger</t>
   </si>
 </sst>
 </file>
@@ -519,12 +519,19 @@
     <numFmt numFmtId="170" formatCode="0.0%"/>
     <numFmt numFmtId="171" formatCode="0.0000000%"/>
   </numFmts>
-  <fonts count="35">
+  <fonts count="36">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Lettertype hoofdtekst"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1059,550 +1066,551 @@
   </borders>
   <cellStyleXfs count="288">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="32" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="182">
+  <cellXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="24" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="20" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="29" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="29" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="30" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="30" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="31" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="29" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="17" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="20" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="1" fontId="18" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="28" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="28" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="29" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="29" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="28" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="17" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="18" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="10" fillId="2" borderId="0" xfId="287" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="11" fillId="2" borderId="0" xfId="287" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="29" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" xfId="259" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="5" xfId="259" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="259" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="5" xfId="259" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="28" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="28" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="29" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="29" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="34" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="34" fillId="0" borderId="18" xfId="287" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="34" fillId="2" borderId="18" xfId="287" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="35" fillId="0" borderId="18" xfId="287" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="35" fillId="2" borderId="18" xfId="287" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="31" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="22" fillId="2" borderId="0" xfId="259" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="288">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -3125,7 +3133,7 @@
   <dimension ref="B2:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="16"/>
@@ -3144,38 +3152,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="16" customHeight="1">
-      <c r="B2" s="167" t="s">
+      <c r="B2" s="173" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="168"/>
-      <c r="D2" s="168"/>
-      <c r="E2" s="168"/>
-      <c r="F2" s="168"/>
-      <c r="G2" s="169"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="175"/>
     </row>
     <row r="3" spans="2:10">
-      <c r="B3" s="170"/>
-      <c r="C3" s="171"/>
-      <c r="D3" s="171"/>
-      <c r="E3" s="171"/>
-      <c r="F3" s="171"/>
-      <c r="G3" s="172"/>
+      <c r="B3" s="176"/>
+      <c r="C3" s="177"/>
+      <c r="D3" s="177"/>
+      <c r="E3" s="177"/>
+      <c r="F3" s="177"/>
+      <c r="G3" s="178"/>
     </row>
     <row r="4" spans="2:10">
-      <c r="B4" s="170"/>
-      <c r="C4" s="171"/>
-      <c r="D4" s="171"/>
-      <c r="E4" s="171"/>
-      <c r="F4" s="171"/>
-      <c r="G4" s="172"/>
+      <c r="B4" s="176"/>
+      <c r="C4" s="177"/>
+      <c r="D4" s="177"/>
+      <c r="E4" s="177"/>
+      <c r="F4" s="177"/>
+      <c r="G4" s="178"/>
     </row>
     <row r="5" spans="2:10">
-      <c r="B5" s="173"/>
-      <c r="C5" s="174"/>
-      <c r="D5" s="174"/>
-      <c r="E5" s="174"/>
-      <c r="F5" s="174"/>
-      <c r="G5" s="175"/>
+      <c r="B5" s="179"/>
+      <c r="C5" s="180"/>
+      <c r="D5" s="180"/>
+      <c r="E5" s="180"/>
+      <c r="F5" s="180"/>
+      <c r="G5" s="181"/>
     </row>
     <row r="6" spans="2:10" ht="17" thickBot="1"/>
     <row r="7" spans="2:10">
@@ -3295,7 +3303,7 @@
       </c>
       <c r="E14" s="138">
         <f>'Research data'!E10</f>
-        <v>0.115</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="F14" s="137"/>
       <c r="G14" s="137"/>
@@ -3315,7 +3323,7 @@
       </c>
       <c r="E15" s="138">
         <f>'Research data'!E11</f>
-        <v>0.115</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="F15" s="137"/>
       <c r="G15" s="137"/>
@@ -3339,7 +3347,7 @@
       <c r="F16" s="137"/>
       <c r="G16" s="137"/>
       <c r="H16" s="137"/>
-      <c r="I16" s="176" t="s">
+      <c r="I16" s="167" t="s">
         <v>132</v>
       </c>
       <c r="J16" s="143"/>
@@ -3527,7 +3535,7 @@
         <v>0.04</v>
       </c>
       <c r="F27" s="137"/>
-      <c r="G27" s="178" t="s">
+      <c r="G27" s="169" t="s">
         <v>136</v>
       </c>
       <c r="H27" s="137"/>
@@ -3597,26 +3605,26 @@
       </c>
       <c r="J31" s="81"/>
     </row>
-    <row r="32" spans="2:10" s="180" customFormat="1" ht="17" thickBot="1">
-      <c r="B32" s="177"/>
-      <c r="C32" s="178" t="s">
+    <row r="32" spans="2:10" s="171" customFormat="1" ht="17" thickBot="1">
+      <c r="B32" s="168"/>
+      <c r="C32" s="169" t="s">
         <v>133</v>
       </c>
       <c r="D32" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E32" s="181">
+      <c r="E32" s="172">
         <v>0</v>
       </c>
-      <c r="F32" s="178"/>
-      <c r="G32" s="178" t="s">
+      <c r="F32" s="169"/>
+      <c r="G32" s="169" t="s">
         <v>134</v>
       </c>
-      <c r="H32" s="178"/>
-      <c r="I32" s="176" t="s">
+      <c r="H32" s="169"/>
+      <c r="I32" s="167" t="s">
         <v>135</v>
       </c>
-      <c r="J32" s="179"/>
+      <c r="J32" s="170"/>
     </row>
     <row r="33" spans="2:10" ht="17" thickBot="1">
       <c r="B33" s="32"/>
@@ -3632,7 +3640,7 @@
       <c r="F33" s="31"/>
       <c r="G33" s="31"/>
       <c r="H33" s="31"/>
-      <c r="I33" s="176" t="s">
+      <c r="I33" s="167" t="s">
         <v>132</v>
       </c>
       <c r="J33" s="81"/>
@@ -3824,11 +3832,11 @@
       </c>
       <c r="E10" s="139">
         <f t="shared" ref="E10:E11" si="0">I10</f>
-        <v>0.115</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="I10" s="139">
         <f>Notes!E114</f>
-        <v>0.115</v>
+        <v>1.0999999999999999E-2</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="141" customFormat="1" ht="17" thickBot="1">
@@ -3841,11 +3849,11 @@
       </c>
       <c r="E11" s="139">
         <f t="shared" si="0"/>
-        <v>0.115</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="I11" s="139">
         <f>Notes!E115</f>
-        <v>0.115</v>
+        <v>1.0999999999999999E-2</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -3928,7 +3936,7 @@
   <dimension ref="B1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20:G21"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="33.140625" defaultRowHeight="16"/>
@@ -4170,7 +4178,7 @@
       <c r="H16" s="166" t="s">
         <v>128</v>
       </c>
-      <c r="I16" s="166" t="s">
+      <c r="I16" s="182" t="s">
         <v>130</v>
       </c>
     </row>
@@ -4220,6 +4228,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I7" r:id="rId1" xr:uid="{FF867D6F-9A3A-DE4A-BD1B-3592A4204C15}"/>
+    <hyperlink ref="I16" r:id="rId2" display="https://www.ford.nl/bedrijfswagens-en-pickups/e-transit?searchid=ppc:Search_NL(dut)%7C%5BAO%5D_Retail_SD_Generics_Electric_CV_CPPI_EUR%7CShp-T2%7CExact%7Bv1.9%7D:Electric_CV_Car:elektrische%20bestelwagen:b:c:g:GOOGLE&amp;gclid=Cj0KCQiA5NSdBhDfARIsALzs2EAjGwGNHizQrX4_Yqi7qbXx-IkFjglcE_3oBIq6y5sjbu7XNzZ-YS0aApTgEALw_wcB&amp;gclsrc=aw.ds" xr:uid="{C913A878-4B51-774A-9ED8-331D69A2FDD3}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4230,8 +4239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AG199"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="G111" sqref="G111"/>
+    <sheetView topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="G114" sqref="G114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="16"/>
@@ -5011,7 +5020,7 @@
         <v>87</v>
       </c>
       <c r="E113" s="160">
-        <v>115</v>
+        <v>11</v>
       </c>
       <c r="F113" s="161" t="s">
         <v>117</v>
@@ -5051,7 +5060,7 @@
       <c r="C114" s="141"/>
       <c r="E114" s="160">
         <f>E113/1000</f>
-        <v>0.115</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="F114" s="161" t="s">
         <v>88</v>
@@ -5092,7 +5101,7 @@
       </c>
       <c r="E115" s="162">
         <f>E114</f>
-        <v>0.115</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="F115" s="161" t="s">
         <v>88</v>
@@ -5249,7 +5258,7 @@
     </row>
     <row r="123" spans="2:33" s="141" customFormat="1" ht="17" thickBot="1">
       <c r="B123" s="142"/>
-      <c r="D123" s="180" t="s">
+      <c r="D123" s="171" t="s">
         <v>138</v>
       </c>
       <c r="E123" s="163">

</xml_diff>